<commit_message>
Deploying to gh-pages from @ Healthedata1/USCDI5-Sandbox@36db9d45fbe96d16b223f17c9227a32cd5bba28b 🚀
</commit_message>
<xml_diff>
--- a/ValueSet-us-core-clinical-note-type.xlsx
+++ b/ValueSet-us-core-clinical-note-type.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
   <si>
     <t>Property</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t>11504-8</t>
+  </si>
+  <si>
+    <t>34111-5</t>
   </si>
   <si>
     <t/>
@@ -393,7 +396,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -469,16 +472,22 @@
       <c r="A11" t="s" s="2">
         <v>37</v>
       </c>
-      <c r="B11" t="s" s="2">
-        <v>37</v>
-      </c>
+      <c r="B11" s="2"/>
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
         <v>38</v>
       </c>
       <c r="B12" t="s" s="2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="2">
         <v>39</v>
+      </c>
+      <c r="B13" t="s" s="2">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ Healthedata1/USCDI5-Sandbox@ea0c3678f0151cd2596e4fa17b6b55ea6dc2be84 🚀
</commit_message>
<xml_diff>
--- a/ValueSet-us-core-clinical-note-type.xlsx
+++ b/ValueSet-us-core-clinical-note-type.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
   <si>
     <t>Property</t>
   </si>
@@ -127,6 +127,9 @@
   </si>
   <si>
     <t>34111-5</t>
+  </si>
+  <si>
+    <t>42348-3</t>
   </si>
   <si>
     <t/>
@@ -396,7 +399,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -478,16 +481,22 @@
       <c r="A12" t="s" s="2">
         <v>38</v>
       </c>
-      <c r="B12" t="s" s="2">
-        <v>38</v>
-      </c>
+      <c r="B12" s="2"/>
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
         <v>39</v>
       </c>
       <c r="B13" t="s" s="2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s" s="2">
         <v>40</v>
+      </c>
+      <c r="B14" t="s" s="2">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ Healthedata1/USCDI5-Sandbox@f8c87d5727e28ba2cd7eb2ae75d121802cfa3919 🚀
</commit_message>
<xml_diff>
--- a/ValueSet-us-core-clinical-note-type.xlsx
+++ b/ValueSet-us-core-clinical-note-type.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
   <si>
     <t>Property</t>
   </si>
@@ -136,9 +136,6 @@
   </si>
   <si>
     <t>34111-5</t>
-  </si>
-  <si>
-    <t>42348-3</t>
   </si>
   <si>
     <t/>
@@ -424,7 +421,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -506,22 +503,16 @@
       <c r="A12" t="s" s="2">
         <v>41</v>
       </c>
-      <c r="B12" s="2"/>
+      <c r="B12" t="s" s="2">
+        <v>41</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
         <v>42</v>
       </c>
       <c r="B13" t="s" s="2">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s" s="2">
         <v>43</v>
-      </c>
-      <c r="B14" t="s" s="2">
-        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>